<commit_message>
update licenseDraft and testresults
</commit_message>
<xml_diff>
--- a/perftest/testresult.xlsx
+++ b/perftest/testresult.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sai030/Desktop/Data61/ai-copyright-framework-test/perftest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1B920EE-4C96-F04C-A828-151A1775886C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DDE4A49-FFB7-994A-9CA6-37C86063A76B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7600" yWindow="500" windowWidth="19680" windowHeight="17500" activeTab="1" xr2:uid="{26F27A29-B218-EA41-8AFF-639A6F2024A1}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="28300" activeTab="4" xr2:uid="{26F27A29-B218-EA41-8AFF-639A6F2024A1}"/>
   </bookViews>
   <sheets>
     <sheet name="model chain depth (m)" sheetId="1" r:id="rId1"/>
-    <sheet name="training datasets (t) - " sheetId="4" r:id="rId2"/>
+    <sheet name="training datasets (t)" sheetId="4" r:id="rId2"/>
     <sheet name="scraped datasets (d)" sheetId="3" r:id="rId3"/>
     <sheet name="model owners (n)" sheetId="5" r:id="rId4"/>
     <sheet name="licenses (l)" sheetId="6" r:id="rId5"/>
@@ -101,9 +101,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -156,13 +155,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>getModelLicenses:</a:t>
+              <a:t>getModelLicenses</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> execution time vs model chain depth</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -412,13 +406,8 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Model Chain</a:t>
+                  <a:t>Number of models in the model chain (M)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Depth</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -536,7 +525,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Execution Time (ms)</a:t>
+                  <a:t>Execution time (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -986,7 +975,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> of model owners</a:t>
+                  <a:t> of model owners (N)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -1069,6 +1058,7 @@
         <c:axId val="1049987135"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -1557,7 +1547,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> of mdoel owners</a:t>
+                  <a:t> of mdoel owners (N)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -1640,6 +1630,7 @@
         <c:axId val="714748000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2128,7 +2119,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> owners</a:t>
+                  <a:t> owners (N)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -2211,6 +2202,7 @@
         <c:axId val="1049930575"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1000"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -2674,6 +2666,66 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Number of licenses / model</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-GB" baseline="0"/>
+                  <a:t> owner (L)</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-GB"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2739,6 +2791,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB"/>
+                  <a:t>Execution time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3130,6 +3237,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of licenses / model owner (L)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3195,6 +3364,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Execution time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3586,6 +3817,68 @@
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of licenses / model owner (L)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3634,6 +3927,7 @@
         <c:axId val="1020472160"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -3651,6 +3945,68 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Execution time (ms)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3787,7 +4143,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>getModelDatasets: execution time vs model chain depth</a:t>
+              <a:t>getModelDatasets</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4051,8 +4407,15 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Model Chain Depth</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of models in the model chain (M)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4175,7 +4538,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> Time (ms)</a:t>
+                  <a:t> time (ms)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -4346,7 +4709,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>getModelsByLicense: execution time vs model chain depth</a:t>
+              <a:t>getModelsByLicense</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -4610,8 +4973,15 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Model Chain Depth</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of models in the model chain (M)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -4730,7 +5100,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Execution Time</a:t>
+                  <a:t>Execution time</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
@@ -4965,7 +5335,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'training datasets (t) - '!$C$2:$C$11</c:f>
+                <c:f>'training datasets (t)'!$C$2:$C$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="10"/>
@@ -5004,7 +5374,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'training datasets (t) - '!$C$2:$C$11</c:f>
+                <c:f>'training datasets (t)'!$C$2:$C$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="10"/>
@@ -5057,7 +5427,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>'training datasets (t) - '!$A$2:$A$11</c:f>
+              <c:f>'training datasets (t)'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5096,7 +5466,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'training datasets (t) - '!$B$2:$B$11</c:f>
+              <c:f>'training datasets (t)'!$B$2:$B$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5185,7 +5555,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> datasets / model</a:t>
+                  <a:t> datasets / model (T)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -5536,7 +5906,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'training datasets (t) - '!$G$2:$G$11</c:f>
+                <c:f>'training datasets (t)'!$G$2:$G$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="10"/>
@@ -5575,7 +5945,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'training datasets (t) - '!$G$2:$G$11</c:f>
+                <c:f>'training datasets (t)'!$G$2:$G$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="10"/>
@@ -5628,7 +5998,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>'training datasets (t) - '!$A$2:$A$11</c:f>
+              <c:f>'training datasets (t)'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5667,7 +6037,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'training datasets (t) - '!$F$2:$F$11</c:f>
+              <c:f>'training datasets (t)'!$F$2:$F$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -5759,7 +6129,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Number of training datasets / model</a:t>
+                  <a:t>Number of training datasets / model (T)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6109,7 +6479,7 @@
             <c:noEndCap val="0"/>
             <c:plus>
               <c:numRef>
-                <c:f>'training datasets (t) - '!$E$2:$E$11</c:f>
+                <c:f>'training datasets (t)'!$E$2:$E$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="10"/>
@@ -6148,7 +6518,7 @@
             </c:plus>
             <c:minus>
               <c:numRef>
-                <c:f>'training datasets (t) - '!$E$2:$E$11</c:f>
+                <c:f>'training datasets (t)'!$E$2:$E$11</c:f>
                 <c:numCache>
                   <c:formatCode>General</c:formatCode>
                   <c:ptCount val="10"/>
@@ -6201,7 +6571,7 @@
           </c:errBars>
           <c:cat>
             <c:numRef>
-              <c:f>'training datasets (t) - '!$A$2:$A$11</c:f>
+              <c:f>'training datasets (t)'!$A$2:$A$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6240,7 +6610,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>'training datasets (t) - '!$D$2:$D$11</c:f>
+              <c:f>'training datasets (t)'!$D$2:$D$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="10"/>
@@ -6332,7 +6702,7 @@
                       </a:sysClr>
                     </a:solidFill>
                   </a:rPr>
-                  <a:t>Number of training datasets / model</a:t>
+                  <a:t>Number of training datasets / model (T)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -6608,12 +6978,9 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>getModelLicenses:</a:t>
+              <a:t>getModelLicenses</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> execution time vs scraped datasets</a:t>
-            </a:r>
+            <a:endParaRPr lang="en-GB" baseline="0"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -6902,11 +7269,11 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Number of Scraped Datasets</a:t>
+                  <a:t>Number of scraped datasets</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> / Model Owner</a:t>
+                  <a:t> / model owner (D)</a:t>
                 </a:r>
                 <a:endParaRPr lang="en-GB"/>
               </a:p>
@@ -7027,7 +7394,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Execution Time (ms)</a:t>
+                  <a:t>Execution time (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -7187,7 +7554,7 @@
             </a:r>
             <a:r>
               <a:rPr lang="en-GB" baseline="0"/>
-              <a:t>License: execution time vs scraped datasets</a:t>
+              <a:t>License</a:t>
             </a:r>
             <a:endParaRPr lang="en-GB"/>
           </a:p>
@@ -7477,14 +7844,16 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Number</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of scraped datasets / model owner (D)</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> of Scraped Datasets / Model Owner</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
               </a:p>
             </c:rich>
           </c:tx>
@@ -7603,7 +7972,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Execution Time (ms)</a:t>
+                  <a:t>Execution time (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -7759,13 +8128,8 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-GB"/>
-              <a:t>getModelDatasets: execution</a:t>
+              <a:t>getModelDatasets</a:t>
             </a:r>
-            <a:r>
-              <a:rPr lang="en-GB" baseline="0"/>
-              <a:t> time vs scraped datasets</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-GB"/>
           </a:p>
         </c:rich>
       </c:tx>
@@ -8053,8 +8417,15 @@
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Number of Scraped Datasets / Model Owner</a:t>
+                  <a:rPr lang="en-GB" sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:sysClr val="windowText" lastClr="000000">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:sysClr>
+                    </a:solidFill>
+                  </a:rPr>
+                  <a:t>Number of scraped datasets / model owner (D)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -8174,7 +8545,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-GB"/>
-                  <a:t>Execution Time (ms)</a:t>
+                  <a:t>Execution time (ms)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -16444,16 +16815,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>11465</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>15302</xdr:rowOff>
+      <xdr:rowOff>11879</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>4</xdr:col>
-      <xdr:colOff>1354667</xdr:colOff>
-      <xdr:row>37</xdr:row>
-      <xdr:rowOff>16933</xdr:rowOff>
+      <xdr:colOff>1452880</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>20320</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -16557,16 +16928,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>298450</xdr:colOff>
-      <xdr:row>12</xdr:row>
-      <xdr:rowOff>158750</xdr:rowOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12414</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>10011</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>742950</xdr:colOff>
+      <xdr:colOff>1280698</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:rowOff>114357</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -17304,8 +17675,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DDD8F8DA-3E33-9A4B-BD49-45C7476A6493}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="50" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+    <sheetView topLeftCell="A5" zoomScale="125" workbookViewId="0">
+      <selection activeCell="E42" sqref="E42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17602,10 +17973,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E6C320B-C7F9-AB46-A571-6B08986463EC}">
-  <dimension ref="A1:Q78"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="50" workbookViewId="0">
-      <selection activeCell="Q78" sqref="Q78"/>
+    <sheetView zoomScale="111" zoomScaleNormal="111" workbookViewId="0">
+      <selection activeCell="I46" sqref="I46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -17889,9 +18260,6 @@
       <c r="G11">
         <v>51.8</v>
       </c>
-    </row>
-    <row r="78" spans="17:17" x14ac:dyDescent="0.2">
-      <c r="Q78" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -17903,8 +18271,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D69B70CE-4620-4847-BCF8-B8FDB88F4A67}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="62" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+    <sheetView zoomScale="164" workbookViewId="0">
+      <selection activeCell="H37" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18199,8 +18567,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADF02CF6-D7EB-0048-8624-5ED56F87871A}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="64" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView zoomScale="142" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -18492,8 +18860,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D996F402-66D9-D348-9DFC-6D4E71AF19F9}">
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView zoomScale="65" workbookViewId="0">
-      <selection activeCell="J35" sqref="J35"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>